<commit_message>
user requirements are the best
</commit_message>
<xml_diff>
--- a/thatAccessFileOfDoom/DriverDBQuestionsAndAnswers.xlsx
+++ b/thatAccessFileOfDoom/DriverDBQuestionsAndAnswers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrause\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkrause\Documents\CodeMe\Mysql\thatAccessFileOfDoom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{941C011F-CF75-484E-BB35-BF06B22C5D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDBFC66-C9C3-45CA-9938-8567D4DBCA1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{8DDC69CF-C9A9-4FB2-BA86-607A5EC29FD2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8DDC69CF-C9A9-4FB2-BA86-607A5EC29FD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="176">
   <si>
     <t>Tables</t>
   </si>
@@ -563,13 +563,16 @@
   </si>
   <si>
     <t>INSURANCE PRORATE INCLUDES WEEKEND</t>
+  </si>
+  <si>
+    <t>should be same as driver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -577,13 +580,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -598,8 +614,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,425 +1036,427 @@
   <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N6" t="s">
+      <c r="N6" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="B43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="B44" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1452,62 +1471,63 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1520,198 +1540,204 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839739C5-14EE-41FC-B8B4-A3832CBF51AE}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="1" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="1" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
+      <c r="J14" s="1" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J16" t="s">
+      <c r="J16" s="1" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="20" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J20" s="1" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="22" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1725,59 +1751,61 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1785,156 +1813,158 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50227565-450C-4BEE-857C-9937F1DBA645}">
   <dimension ref="B1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="1" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1948,24 +1978,26 @@
   <dimension ref="B2:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="1" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="10.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>158</v>
       </c>
     </row>

</xml_diff>